<commit_message>
Some dates had an incorrect year
</commit_message>
<xml_diff>
--- a/Tests/Validation/Wheat/data/FAR RRC W21-03.xlsx
+++ b/Tests/Validation/Wheat/data/FAR RRC W21-03.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\ApsimX\Tests\Validation\Wheat\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E62528AF-FD84-4A70-AF24-591A56525E5E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{941C1005-ADB5-4714-A283-F9BD4E4919CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16896" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -566,12 +566,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AB245"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="AE14" sqref="AE14"/>
+    <sheetView tabSelected="1" topLeftCell="A106" workbookViewId="0">
+      <selection activeCell="C118" sqref="C118"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
+    <col min="2" max="2" width="14.44140625" customWidth="1"/>
+    <col min="3" max="3" width="17.109375" customWidth="1"/>
     <col min="23" max="23" width="7.77734375" customWidth="1"/>
   </cols>
   <sheetData>
@@ -850,7 +852,7 @@
         <v>28</v>
       </c>
       <c r="B10" s="1">
-        <v>44867</v>
+        <v>44502</v>
       </c>
       <c r="D10" t="s">
         <v>29</v>
@@ -873,7 +875,7 @@
         <v>28</v>
       </c>
       <c r="B11" s="1">
-        <v>44917</v>
+        <v>44552</v>
       </c>
       <c r="C11" t="s">
         <v>32</v>
@@ -1149,7 +1151,7 @@
         <v>33</v>
       </c>
       <c r="B20" s="1">
-        <v>44867</v>
+        <v>44502</v>
       </c>
       <c r="D20" t="s">
         <v>29</v>
@@ -1172,7 +1174,7 @@
         <v>33</v>
       </c>
       <c r="B21" s="1">
-        <v>44917</v>
+        <v>44552</v>
       </c>
       <c r="C21" t="s">
         <v>32</v>
@@ -1448,7 +1450,7 @@
         <v>35</v>
       </c>
       <c r="B30" s="1">
-        <v>44867</v>
+        <v>44502</v>
       </c>
       <c r="D30" t="s">
         <v>29</v>
@@ -1471,7 +1473,7 @@
         <v>35</v>
       </c>
       <c r="B31" s="1">
-        <v>44908</v>
+        <v>44543</v>
       </c>
       <c r="C31" t="s">
         <v>32</v>
@@ -1500,7 +1502,7 @@
         <v>35</v>
       </c>
       <c r="B32" s="1">
-        <v>44917</v>
+        <v>44552</v>
       </c>
       <c r="C32" t="s">
         <v>32</v>
@@ -1770,7 +1772,7 @@
         <v>37</v>
       </c>
       <c r="B41" s="1">
-        <v>44867</v>
+        <v>44502</v>
       </c>
       <c r="D41" t="s">
         <v>29</v>
@@ -1793,7 +1795,7 @@
         <v>37</v>
       </c>
       <c r="B42" s="1">
-        <v>44908</v>
+        <v>44543</v>
       </c>
       <c r="C42" t="s">
         <v>32</v>
@@ -1822,7 +1824,7 @@
         <v>37</v>
       </c>
       <c r="B43" s="1">
-        <v>44917</v>
+        <v>44552</v>
       </c>
       <c r="C43" t="s">
         <v>32</v>
@@ -2092,7 +2094,7 @@
         <v>39</v>
       </c>
       <c r="B52" s="1">
-        <v>44867</v>
+        <v>44502</v>
       </c>
       <c r="D52" t="s">
         <v>29</v>
@@ -2115,7 +2117,7 @@
         <v>39</v>
       </c>
       <c r="B53" s="1">
-        <v>44908</v>
+        <v>44543</v>
       </c>
       <c r="C53" t="s">
         <v>32</v>
@@ -2144,7 +2146,7 @@
         <v>39</v>
       </c>
       <c r="B54" s="1">
-        <v>44917</v>
+        <v>44552</v>
       </c>
       <c r="C54" t="s">
         <v>32</v>
@@ -2414,7 +2416,7 @@
         <v>41</v>
       </c>
       <c r="B63" s="1">
-        <v>44867</v>
+        <v>44502</v>
       </c>
       <c r="D63" t="s">
         <v>29</v>
@@ -2437,7 +2439,7 @@
         <v>41</v>
       </c>
       <c r="B64" s="1">
-        <v>44917</v>
+        <v>44552</v>
       </c>
       <c r="C64" t="s">
         <v>32</v>
@@ -2713,7 +2715,7 @@
         <v>43</v>
       </c>
       <c r="B73" s="1">
-        <v>44867</v>
+        <v>44502</v>
       </c>
       <c r="D73" t="s">
         <v>29</v>
@@ -2736,7 +2738,7 @@
         <v>43</v>
       </c>
       <c r="B74" s="1">
-        <v>44917</v>
+        <v>44552</v>
       </c>
       <c r="C74" t="s">
         <v>32</v>
@@ -3064,7 +3066,7 @@
         <v>45</v>
       </c>
       <c r="B85" s="1">
-        <v>44867</v>
+        <v>44502</v>
       </c>
       <c r="D85" t="s">
         <v>46</v>
@@ -3087,7 +3089,7 @@
         <v>45</v>
       </c>
       <c r="B86" s="1">
-        <v>44917</v>
+        <v>44552</v>
       </c>
       <c r="C86" t="s">
         <v>32</v>
@@ -3415,7 +3417,7 @@
         <v>48</v>
       </c>
       <c r="B97" s="1">
-        <v>44867</v>
+        <v>44502</v>
       </c>
       <c r="D97" t="s">
         <v>46</v>
@@ -3438,7 +3440,7 @@
         <v>48</v>
       </c>
       <c r="B98" s="1">
-        <v>44908</v>
+        <v>44543</v>
       </c>
       <c r="C98" t="s">
         <v>32</v>
@@ -3467,7 +3469,7 @@
         <v>48</v>
       </c>
       <c r="B99" s="1">
-        <v>44917</v>
+        <v>44552</v>
       </c>
       <c r="C99" t="s">
         <v>32</v>
@@ -3789,7 +3791,7 @@
         <v>49</v>
       </c>
       <c r="B110" s="1">
-        <v>44867</v>
+        <v>44502</v>
       </c>
       <c r="D110" t="s">
         <v>46</v>
@@ -3812,7 +3814,7 @@
         <v>49</v>
       </c>
       <c r="B111" s="1">
-        <v>44917</v>
+        <v>44552</v>
       </c>
       <c r="C111" t="s">
         <v>32</v>
@@ -4140,7 +4142,7 @@
         <v>50</v>
       </c>
       <c r="B122" s="1">
-        <v>44867</v>
+        <v>44502</v>
       </c>
       <c r="D122" t="s">
         <v>46</v>
@@ -4163,7 +4165,7 @@
         <v>50</v>
       </c>
       <c r="B123" s="1">
-        <v>44908</v>
+        <v>44543</v>
       </c>
       <c r="C123" t="s">
         <v>32</v>
@@ -4192,7 +4194,7 @@
         <v>50</v>
       </c>
       <c r="B124" s="1">
-        <v>44917</v>
+        <v>44552</v>
       </c>
       <c r="C124" t="s">
         <v>32</v>
@@ -4514,7 +4516,7 @@
         <v>51</v>
       </c>
       <c r="B135" s="1">
-        <v>44867</v>
+        <v>44502</v>
       </c>
       <c r="D135" t="s">
         <v>46</v>
@@ -4537,7 +4539,7 @@
         <v>51</v>
       </c>
       <c r="B136" s="1">
-        <v>44917</v>
+        <v>44552</v>
       </c>
       <c r="C136" t="s">
         <v>32</v>
@@ -4865,7 +4867,7 @@
         <v>52</v>
       </c>
       <c r="B147" s="1">
-        <v>44867</v>
+        <v>44502</v>
       </c>
       <c r="D147" t="s">
         <v>46</v>
@@ -4888,7 +4890,7 @@
         <v>52</v>
       </c>
       <c r="B148" s="1">
-        <v>44908</v>
+        <v>44543</v>
       </c>
       <c r="C148" t="s">
         <v>32</v>
@@ -4917,7 +4919,7 @@
         <v>52</v>
       </c>
       <c r="B149" s="1">
-        <v>44917</v>
+        <v>44552</v>
       </c>
       <c r="C149" t="s">
         <v>32</v>
@@ -5239,7 +5241,7 @@
         <v>53</v>
       </c>
       <c r="B160" s="1">
-        <v>44867</v>
+        <v>44502</v>
       </c>
       <c r="D160" t="s">
         <v>46</v>
@@ -5262,7 +5264,7 @@
         <v>53</v>
       </c>
       <c r="B161" s="1">
-        <v>44917</v>
+        <v>44552</v>
       </c>
       <c r="C161" t="s">
         <v>32</v>
@@ -5564,7 +5566,7 @@
         <v>54</v>
       </c>
       <c r="B171" s="1">
-        <v>44866</v>
+        <v>44501</v>
       </c>
       <c r="D171" t="s">
         <v>55</v>
@@ -5590,7 +5592,7 @@
         <v>54</v>
       </c>
       <c r="B172" s="1">
-        <v>44867</v>
+        <v>44502</v>
       </c>
       <c r="D172" t="s">
         <v>55</v>
@@ -5613,7 +5615,7 @@
         <v>54</v>
       </c>
       <c r="B173" s="1">
-        <v>44917</v>
+        <v>44552</v>
       </c>
       <c r="C173" t="s">
         <v>32</v>
@@ -5921,7 +5923,7 @@
         <v>57</v>
       </c>
       <c r="B183" s="1">
-        <v>44867</v>
+        <v>44502</v>
       </c>
       <c r="D183" t="s">
         <v>55</v>
@@ -5944,7 +5946,7 @@
         <v>57</v>
       </c>
       <c r="B184" s="1">
-        <v>44908</v>
+        <v>44543</v>
       </c>
       <c r="C184" t="s">
         <v>32</v>
@@ -5973,7 +5975,7 @@
         <v>57</v>
       </c>
       <c r="B185" s="1">
-        <v>44917</v>
+        <v>44552</v>
       </c>
       <c r="C185" t="s">
         <v>32</v>
@@ -6269,7 +6271,7 @@
         <v>58</v>
       </c>
       <c r="B195" s="1">
-        <v>44866</v>
+        <v>44501</v>
       </c>
       <c r="D195" t="s">
         <v>55</v>
@@ -6295,7 +6297,7 @@
         <v>58</v>
       </c>
       <c r="B196" s="1">
-        <v>44867</v>
+        <v>44502</v>
       </c>
       <c r="D196" t="s">
         <v>55</v>
@@ -6318,7 +6320,7 @@
         <v>58</v>
       </c>
       <c r="B197" s="1">
-        <v>44917</v>
+        <v>44552</v>
       </c>
       <c r="C197" t="s">
         <v>32</v>
@@ -6626,7 +6628,7 @@
         <v>59</v>
       </c>
       <c r="B207" s="1">
-        <v>44867</v>
+        <v>44502</v>
       </c>
       <c r="D207" t="s">
         <v>55</v>
@@ -6649,7 +6651,7 @@
         <v>59</v>
       </c>
       <c r="B208" s="1">
-        <v>44908</v>
+        <v>44543</v>
       </c>
       <c r="C208" t="s">
         <v>32</v>
@@ -6678,7 +6680,7 @@
         <v>59</v>
       </c>
       <c r="B209" s="1">
-        <v>44917</v>
+        <v>44552</v>
       </c>
       <c r="C209" t="s">
         <v>32</v>
@@ -6980,7 +6982,7 @@
         <v>60</v>
       </c>
       <c r="B219" s="1">
-        <v>44867</v>
+        <v>44502</v>
       </c>
       <c r="D219" t="s">
         <v>55</v>
@@ -7003,7 +7005,7 @@
         <v>60</v>
       </c>
       <c r="B220" s="1">
-        <v>44908</v>
+        <v>44543</v>
       </c>
       <c r="C220" t="s">
         <v>32</v>
@@ -7032,7 +7034,7 @@
         <v>60</v>
       </c>
       <c r="B221" s="1">
-        <v>44917</v>
+        <v>44552</v>
       </c>
       <c r="C221" t="s">
         <v>32</v>
@@ -7328,7 +7330,7 @@
         <v>61</v>
       </c>
       <c r="B231" s="1">
-        <v>44866</v>
+        <v>44501</v>
       </c>
       <c r="D231" t="s">
         <v>55</v>
@@ -7354,7 +7356,7 @@
         <v>61</v>
       </c>
       <c r="B232" s="1">
-        <v>44867</v>
+        <v>44502</v>
       </c>
       <c r="D232" t="s">
         <v>55</v>
@@ -7377,7 +7379,7 @@
         <v>61</v>
       </c>
       <c r="B233" s="1">
-        <v>44917</v>
+        <v>44552</v>
       </c>
       <c r="C233" t="s">
         <v>32</v>
@@ -7679,7 +7681,7 @@
         <v>62</v>
       </c>
       <c r="B243" s="1">
-        <v>44866</v>
+        <v>44501</v>
       </c>
       <c r="D243" t="s">
         <v>55</v>
@@ -7705,7 +7707,7 @@
         <v>62</v>
       </c>
       <c r="B244" s="1">
-        <v>44867</v>
+        <v>44502</v>
       </c>
       <c r="D244" t="s">
         <v>55</v>
@@ -7728,7 +7730,7 @@
         <v>62</v>
       </c>
       <c r="B245" s="1">
-        <v>44917</v>
+        <v>44552</v>
       </c>
       <c r="C245" t="s">
         <v>32</v>

</xml_diff>